<commit_message>
updated file paths + fixed level counter
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -943,7 +943,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1033,7 +1033,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>G0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1067,175 +1067,13 @@
         <v>45566.25</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="N2" t="n">
         <v>10080</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>17</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H3" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I3" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>30</v>
-      </c>
-      <c r="M3" t="n">
-        <v>3</v>
-      </c>
-      <c r="N3" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>17</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H4" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I4" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N4" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>17</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>G4</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H5" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O5" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1331,21 +1169,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tutorial_video(physical_activity)</t>
+          <t>Take_a_45-minute_walk_without_stopping</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/a4466cf8-adb1-4a54-9e56-075eae837a53.h5p</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -1356,12 +1189,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1369,11 +1202,11 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, o5bnwon9i6rv3nupuntgzsqhywfb0sk7sppsi9mazy5bwu5ph]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 462vw0lmun2sepot3v7vw68yssv5zwetko5hawu]</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1383,11 +1216,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Take_a_45-minute_walk_without_stopping</t>
+          <t>Cook_dinner_for_someone</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1416,11 +1249,11 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 60szg8o5o8]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, hbeifsnlhqqe8x9ioeittpnkmo7dgd8uh1oj]</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1430,11 +1263,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Take_200_steps</t>
+          <t>Practice_a_brain_game</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1450,12 +1283,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1463,11 +1296,11 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 3000], [SECRET, EQUAL, ej3dg5z2rq1m6g7v97m]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, v3zyw9ldimbms7mkq6jkbbi7vfnkkm6tgeljwn9jnqfgl97c]</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1477,11 +1310,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Include_10_minutes_of_uphill_walking_during_one_of_your_walks</t>
+          <t>Practice_meditation</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1510,11 +1343,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, h6xgwwhtqnc2gplsy3h1ncqvt09bssdiqxi6rk8cjk9ku8u]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 1iyvk5ukxivygjfi5u7]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1524,11 +1357,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Walk_9000_steps_in_a_day</t>
+          <t>Watch_a_documentary</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1544,12 +1377,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>DAY_AGGREGATE</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>DAY_AGGREGATE</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -1557,11 +1390,11 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[STEPS_SUM, STRICTLY_GREATER, 9000], [SECRET, EQUAL, 1aaukm7ml4g9m8]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, p9295ognntc84730ycyr4w9d0cv2]</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1571,11 +1404,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Walk_9000_steps_in_a_day</t>
+          <t>Practice_a_brain_game</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1591,12 +1424,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>DAY_AGGREGATE</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>DAY_AGGREGATE</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -1604,11 +1437,11 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[STEPS_SUM, STRICTLY_GREATER, 9000], [SECRET, EQUAL, qqj1vx1hq6ndxp5d6q907icqb1zeeh1t7vj81fvypxm]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, i89b482zkonvkwwuop7d8jlmozp2g4hrr5b3aow0v]</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1618,21 +1451,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>tutorial_video(social_activity)</t>
+          <t>Learn_a_new_word</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1643,12 +1471,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -1656,7 +1484,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, dibhlux6stuurubsixtsfnfa5nke6v5kr]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, rulzt8cc6veus9gk0m8f2]</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -1670,11 +1498,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Call_a_friend</t>
+          <t>Do_a_5_min_yoga_session</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1703,11 +1531,11 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 81hceada27ud7qcheqdudbuaqkb]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 77tfljxefohkwa04ctncaiagnqamm9wzjtvyk0c2a5bp]</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1717,11 +1545,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Go_to_a_social_event</t>
+          <t>Take_a_45-minute_walk_without_stopping</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1750,11 +1578,11 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, fa5e6ynirrcd]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, lskr47m4ho2l7axfohifxuef]</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1764,11 +1592,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Call_a_friend</t>
+          <t>Plan_an_event_with_others</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1797,13 +1625,154 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 75lkfq7psmamjg9q65xdy]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, bxa5vnt2er8bgf3cs8]</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N11" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Take_a_45-minute_walk_without_stopping</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>7</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, vs9rzzqb5nzwi74f3dfic7j2unw7h4u7wppvxnw1wf9nl]</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>6</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Practice_creative_writing</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, dn35lmw8ukbdvjwa78vmnyo020omtteih2g5e]</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>6</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Go_on_a_group_activity</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, f54bi81ahqd1t918]</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>5</v>
+      </c>
+      <c r="N14" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
minigames show up in plan
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -23,9 +23,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -943,7 +944,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1066,6 +1067,7 @@
       <c r="I2" s="6" t="n">
         <v>45566.25</v>
       </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
         <v>1</v>
       </c>
@@ -1078,6 +1080,7 @@
       <c r="N2" t="n">
         <v>10080</v>
       </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1117,6 +1120,7 @@
       <c r="I3" s="6" t="n">
         <v>45566.25</v>
       </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>0</v>
       </c>
@@ -1171,6 +1175,7 @@
       <c r="I4" s="6" t="n">
         <v>45566.25</v>
       </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
         <v>0</v>
       </c>
@@ -1225,11 +1230,12 @@
       <c r="I5" s="6" t="n">
         <v>45566.25</v>
       </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
         <v>5</v>
@@ -1279,11 +1285,12 @@
       <c r="I6" s="6" t="n">
         <v>45566.25</v>
       </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M6" t="n">
         <v>6</v>
@@ -1333,17 +1340,74 @@
       <c r="I7" s="6" t="n">
         <v>45566.25</v>
       </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>7</v>
       </c>
       <c r="N7" t="n">
         <v>10080</v>
       </c>
       <c r="O7" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>17</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>TASKS_COLLECTION</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>G7</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Generated by AI</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>45474.25</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>45566.25</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>12</v>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="n">
+        <v>10080</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1443,7 +1507,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tutorial_video(cognitive_activity)</t>
+          <t>tutorial_video(minigame_activity)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1453,7 +1517,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/66972617-5cd5-40e1-8432-ecd99b7dcf10.h5p</t>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -1477,7 +1541,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, zh25jq4a778f9r7ib0xigl50ynahfz5c]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, tqpjhob9xregwy4nfkoatmpjnsfmff]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1529,7 +1593,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, eo6qfa6mcn74fn5z3a6cw2e2iw5w4p4c5pq7ofn41nb4w]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 2a07ecfqm7d7czyv05aq3p4a342bekoflleue45dg]</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -1547,7 +1611,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tutorial_video(social_activity)</t>
+          <t>tutorial_video(cognitive_activity)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1557,7 +1621,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/66972617-5cd5-40e1-8432-ecd99b7dcf10.h5p</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -1581,7 +1645,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 5m5wx6jagmtjrcwwi4uq]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, b1wb72y0eezfwzyere14chjsgksoodqqhgkp2pwzj]</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -1599,12 +1663,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Practice_a_memory_game</t>
+          <t>tutorial_video(social_activity)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -1615,12 +1684,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -1628,11 +1697,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, d0lm74qf5wzacwad60m5f0xifafn9pk]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 0wpp1u7670tr9hssjr70il]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1642,11 +1711,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Put_on_your_walking_shoes_and_take_a_picture_of_them</t>
+          <t>Play_confusing_arrows</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1675,11 +1744,11 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, mynbqzouwkvy]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 5gol73tpopfrl51qczu97obp1ii6u7aus3jytydht2c]</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1689,11 +1758,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Plan_an_event_with_others</t>
+          <t>Take_a_25-minute_walk_without_stopping</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1722,11 +1791,11 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, pkb77gdpe7m4v5s160w09vlf9x14ll5q6]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, tqrp9x8iwem9]</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1740,7 +1809,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Practice_creative_writing</t>
+          <t>Go_on_a_peaceful_walk</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1769,11 +1838,11 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 2xvewqk4zvzysiba6kgrbzm7w4yyqhnjn9a5z9vvjm58]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 93tar0275rnmscvimf2bp9zg4ult2exlsz6uaixhst90qv]</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1787,7 +1856,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Plan_an_event_with_others</t>
+          <t>Call_a_friend</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1816,11 +1885,11 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 9h2fv08aqjcvexno3avzbdf9oc6bo]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, wb9pyyeiwc5y88ux8ibs2n8qv870f57dvn6fc589o]</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1830,11 +1899,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Take_a_15-minute_walk_without_stopping</t>
+          <t>Take_200_steps</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1850,12 +1919,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K10" t="n">
@@ -1863,11 +1932,11 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 0lc2wif91okb018k57x321]</t>
+          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, num1muhnvu0eyzemnofcccc8g76lhq9]</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1881,7 +1950,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Take_a_15-minute_walk_without_stopping</t>
+          <t>Engage_with_others</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1910,11 +1979,11 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, dslzpdprjaw3ob1]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, e2lq1jbckpzyawtdqywj5ingd46p92np5q3xkwygkjlcsu]</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1928,7 +1997,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Go_on_a_group_activity</t>
+          <t>Watch_a_documentary</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1957,11 +2026,11 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 0cge3yxvlojznquf67ydai95xzvp0ilwuqrlz6tpwijwn9wru]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, vp1dng10sjhd8ccqqfc6x21ivta0p6fzj]</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1971,11 +2040,11 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Watch_a_documentary</t>
+          <t>Practice_a_brain_game</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2004,13 +2073,107 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, b6p3l4ls4xq11eb0ip64ywjp51jdcsefm09od35hjeg5y]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, ksazt7vngzbdiqpnbotgit0teal1]</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N13" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Join_a_community_event</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, 86t4e8m8rif8dv7qnwlm6k7ymxcew9x]</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>10</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>7</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Take_100_steps</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>7</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>[STEPS, STRICTLY_GREATER, 100], [SECRET, EQUAL, sc19c4wruvcche8qq89ydo2ntyy1]</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
fixed campaigns outdated issue
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="campaigns" sheetId="1" state="visible" r:id="rId1"/>
@@ -23,12 +23,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -45,6 +44,13 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,10 +76,11 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -81,11 +88,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="1" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -681,13 +690,14 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col width="14" customWidth="1" min="4" max="5"/>
+    <col width="38.8984375" customWidth="1" min="4" max="4"/>
+    <col width="40.09765625" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -730,10 +740,10 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45474.25</v>
+        <v>45658.25</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45565.875</v>
+        <v>45868.875</v>
       </c>
     </row>
   </sheetData>
@@ -944,7 +954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -953,77 +963,77 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>campaign</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>image</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>visualizations</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>start</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>end</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>contender</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>is_initial_level</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>target</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>success_next</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="5" t="inlineStr">
         <is>
           <t>evaluate_fail_every_x_minutes</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="5" t="inlineStr">
         <is>
           <t>failure_next</t>
         </is>
@@ -1061,13 +1071,12 @@
           <t>122</t>
         </is>
       </c>
-      <c r="H2" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I2" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="H2" s="7" t="n">
+        <v>45658.25</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <v>45839.25</v>
+      </c>
       <c r="K2" t="n">
         <v>1</v>
       </c>
@@ -1080,7 +1089,6 @@
       <c r="N2" t="n">
         <v>10080</v>
       </c>
-      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1114,300 +1122,23 @@
           <t>122</t>
         </is>
       </c>
-      <c r="H3" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I3" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="H3" s="7" t="n">
+        <v>45658.25</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>45839.25</v>
+      </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="N3" t="n">
         <v>10080</v>
       </c>
       <c r="O3" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>17</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H4" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I4" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N4" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>17</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>G4</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H5" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>5</v>
-      </c>
-      <c r="N5" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>17</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>G5</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H6" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I6" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>10</v>
-      </c>
-      <c r="M6" t="n">
-        <v>6</v>
-      </c>
-      <c r="N6" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>17</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>G6</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H7" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I7" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>5</v>
-      </c>
-      <c r="M7" t="n">
-        <v>7</v>
-      </c>
-      <c r="N7" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O7" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>17</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>G7</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H8" s="6" t="n">
-        <v>45474.25</v>
-      </c>
-      <c r="I8" s="6" t="n">
-        <v>45566.25</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>12</v>
-      </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O8" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1421,7 +1152,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1430,72 +1161,72 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>challenge</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>image</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>video</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>h5p_slug</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>max_times_fired</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>min_days_between_fire</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>activityscheme_default</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>activityschemes_allowed</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>image_required</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>conditions</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>points</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="5" t="inlineStr">
         <is>
           <t>dataproviders</t>
         </is>
@@ -1541,7 +1272,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, tqpjhob9xregwy4nfkoatmpjnsfmff]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, qhm8ejcqzqi1]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1559,33 +1290,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tutorial_video(physical_activity)</t>
+          <t>Buy half heart</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/a4466cf8-adb1-4a54-9e56-075eae837a53.h5p</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>7</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -1593,11 +1316,11 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 2a07ecfqm7d7czyv05aq3p4a342bekoflleue45dg]</t>
+          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 1], [SECRET, EQUAL, 4p0vowxowbzc0g1enu223q0j7fp25joeap4r6nlm]</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1607,37 +1330,29 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tutorial_video(cognitive_activity)</t>
+          <t>Score 5 points</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/66972617-5cd5-40e1-8432-ecd99b7dcf10.h5p</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>7</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1645,11 +1360,11 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, b1wb72y0eezfwzyere14chjsgksoodqqhgkp2pwzj]</t>
+          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 5],[MINIGAMESTATE_ID, EQUAL, 1], [SECRET, EQUAL, 4kmojhlhkq2auqqg033y0yw]</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1659,37 +1374,29 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>tutorial_video(social_activity)</t>
+          <t>Walk 500 meters</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>7</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -1697,483 +1404,13 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 0wpp1u7670tr9hssjr70il]</t>
+          <t>[DISTANCE, STRICTLY_GREATER, 499], [SECRET, EQUAL, f61ncd1aq6awzlhmnrpygblz9ja1j9pzt3t1nagegfud]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="N5" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Play_confusing_arrows</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 5gol73tpopfrl51qczu97obp1ii6u7aus3jytydht2c]</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Take_a_25-minute_walk_without_stopping</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>7</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, tqrp9x8iwem9]</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Go_on_a_peaceful_walk</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>7</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 93tar0275rnmscvimf2bp9zg4ult2exlsz6uaixhst90qv]</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>2</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Call_a_friend</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>7</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, wb9pyyeiwc5y88ux8ibs2n8qv870f57dvn6fc589o]</t>
-        </is>
-      </c>
-      <c r="M9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Take_200_steps</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>7</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, num1muhnvu0eyzemnofcccc8g76lhq9]</t>
-        </is>
-      </c>
-      <c r="M10" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>6</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Engage_with_others</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" t="n">
-        <v>7</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, e2lq1jbckpzyawtdqywj5ingd46p92np5q3xkwygkjlcsu]</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>6</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Watch_a_documentary</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" t="n">
-        <v>7</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, vp1dng10sjhd8ccqqfc6x21ivta0p6fzj]</t>
-        </is>
-      </c>
-      <c r="M12" t="n">
-        <v>3</v>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>7</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Practice_a_brain_game</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" t="n">
-        <v>7</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, ksazt7vngzbdiqpnbotgit0teal1]</t>
-        </is>
-      </c>
-      <c r="M13" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>7</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Join_a_community_event</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>7</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 86t4e8m8rif8dv7qnwlm6k7ymxcew9x]</t>
-        </is>
-      </c>
-      <c r="M14" t="n">
-        <v>10</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>7</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Take_100_steps</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>7</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>[STEPS, STRICTLY_GREATER, 100], [SECRET, EQUAL, sc19c4wruvcche8qq89ydo2ntyy1]</t>
-        </is>
-      </c>
-      <c r="M15" t="n">
-        <v>1</v>
-      </c>
-      <c r="N15" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
minigames running (no videos)
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -954,7 +954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1044,7 +1044,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>G0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1078,67 +1078,13 @@
         <v>45839.25</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="N2" t="n">
         <v>10080</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>17</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H3" s="7" t="n">
-        <v>45658.25</v>
-      </c>
-      <c r="I3" s="7" t="n">
-        <v>45839.25</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>25</v>
-      </c>
-      <c r="N3" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1234,37 +1180,29 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tutorial_video(minigame_activity)</t>
+          <t>Buy half heart</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/generated-296ffd13/f0a366cc-c574-4807-8dab-5dd53dd47f70.h5p</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>7</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1272,11 +1210,11 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, qhm8ejcqzqi1]</t>
+          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 1]</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1286,11 +1224,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Buy half heart</t>
+          <t>Score 5 points</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1316,11 +1254,11 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 1], [SECRET, EQUAL, 4p0vowxowbzc0g1enu223q0j7fp25joeap4r6nlm]</t>
+          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 5],[MINIGAMESTATE_ID, EQUAL, 1]</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1330,11 +1268,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Score 5 points</t>
+          <t>Walk 500 meters</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1347,12 +1285,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1360,57 +1298,13 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 5],[MINIGAMESTATE_ID, EQUAL, 1], [SECRET, EQUAL, 4kmojhlhkq2auqqg033y0yw]</t>
+          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N4" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Walk 500 meters</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>7</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>[DISTANCE, STRICTLY_GREATER, 499], [SECRET, EQUAL, f61ncd1aq6awzlhmnrpygblz9ja1j9pzt3t1nagegfud]</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>20</v>
-      </c>
-      <c r="N5" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
added minigame support to planner
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -954,7 +954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,13 +1078,121 @@
         <v>45839.25</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>25</v>
       </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
       <c r="N2" t="n">
         <v>10080</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TASKS_COLLECTION</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>G1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Generated by AI</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>45658.25</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>45839.25</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" t="n">
+        <v>10080</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>17</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TASKS_COLLECTION</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Generated by AI</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>45658.25</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>45839.25</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>40</v>
+      </c>
+      <c r="N4" t="n">
+        <v>10080</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1177,6 +1285,61 @@
           <t>dataproviders</t>
         </is>
       </c>
+      <c r="O1" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P1" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q1" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R1" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S1" s="5" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="T1" s="5" t="inlineStr">
+        <is>
+          <t>1.1</t>
+        </is>
+      </c>
+      <c r="U1" s="5" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="V1" s="5" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="W1" s="5" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="X1" s="5" t="inlineStr">
+        <is>
+          <t>2.2</t>
+        </is>
+      </c>
+      <c r="Y1" s="5" t="inlineStr">
+        <is>
+          <t>3.1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1305,6 +1468,364 @@
         <v>20</v>
       </c>
       <c r="N4" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Buy half heart</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>7</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 2]</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>-5</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Score 10 points</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>7</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 10],[MINIGAMESTATE_ID, EQUAL, 2]</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>15</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Walk 500 meters</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>7</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Call a friend/family member</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, fdjklagas37]</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>10</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Buy half heart</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>7</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 3]</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>-5</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Score 20 points</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>7</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>ConfusingArrowsData</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 20],[MINIGAMESTATE_ID, EQUAL, 3]</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>15</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Walk 1500 meters</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>7</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>20</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Call a friend/family member</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>7</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, fdjklagas37]</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>10</v>
+      </c>
+      <c r="N12" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
turned on tutorial feature
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -954,7 +954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1044,7 +1044,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>G0</t>
+          <t>G1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1081,10 +1081,10 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2" t="n">
         <v>10080</v>
@@ -1095,7 +1095,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>G1</t>
+          <t>G2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1132,16 +1132,16 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
         <v>10080</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1149,7 +1149,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>G2</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1186,13 +1186,67 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4</v>
       </c>
       <c r="N4" t="n">
         <v>10080</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>TASKS_COLLECTION</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>G4</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Generated by AI</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>45658.25</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>45839.25</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>40</v>
+      </c>
+      <c r="N5" t="n">
+        <v>10080</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1343,29 +1397,37 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Buy half heart</t>
+          <t>tutorial_video(minigame_activity)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>http://localhost:5173/api/media/media-for-ai-b7b4437a/ba5eb809-ed8e-4688-acb0-0df598a2c57c.h5p</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>7</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1373,11 +1435,11 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 1]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 0anz7bu9mbhbrjwmmnv13bjbtuyc11]</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1387,11 +1449,11 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Score 5 points</t>
+          <t>Buy half heart</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1417,11 +1479,11 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 5],[MINIGAMESTATE_ID, EQUAL, 1]</t>
+          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 1]</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1431,11 +1493,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Walk 500 meters</t>
+          <t>Score 5 points</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1448,12 +1510,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1461,11 +1523,11 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
+          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 5],[MINIGAMESTATE_ID, EQUAL, 1]</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1475,11 +1537,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Buy half heart</t>
+          <t>Walk 500 meters</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1492,12 +1554,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -1505,11 +1567,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 2]</t>
+          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-5</v>
+        <v>20</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1519,11 +1581,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Score 10 points</t>
+          <t>Buy half heart</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1549,11 +1611,11 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 10],[MINIGAMESTATE_ID, EQUAL, 2]</t>
+          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 2]</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>15</v>
+        <v>-5</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1563,11 +1625,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Walk 500 meters</t>
+          <t>Score 10 points</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1580,12 +1642,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -1593,11 +1655,11 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
+          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 10],[MINIGAMESTATE_ID, EQUAL, 2]</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1607,20 +1669,17 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Call a friend/family member</t>
+          <t>Walk 500 meters</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>7</v>
@@ -1640,7 +1699,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, fdjklagas37]</t>
+          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -1654,29 +1713,32 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Buy half heart</t>
+          <t>Call a friend/family member</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>7</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>ConfusingArrowsData</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -1684,11 +1746,11 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 3]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, fdjklagas37]</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1698,11 +1760,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Score 20 points</t>
+          <t>Buy half heart</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1728,11 +1790,11 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 20],[MINIGAMESTATE_ID, EQUAL, 3]</t>
+          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 3]</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>15</v>
+        <v>-5</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1742,11 +1804,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Walk 1500 meters</t>
+          <t>Score 20 points</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1759,12 +1821,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>ConfusingArrowsData</t>
         </is>
       </c>
       <c r="K11" t="n">
@@ -1772,11 +1834,11 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
+          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 20],[MINIGAMESTATE_ID, EQUAL, 3]</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1786,20 +1848,17 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Call a friend/family member</t>
+          <t>Walk 1500 meters</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
         </is>
-      </c>
-      <c r="G12" t="n">
-        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>7</v>
@@ -1819,13 +1878,60 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
+          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>20</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Call a friend/family member</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>WALK</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t xml:space="preserve"> [SECRET, EQUAL, fdjklagas37]</t>
         </is>
       </c>
-      <c r="M12" t="n">
+      <c r="M13" t="n">
         <v>10</v>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
Added fun ratio functionality Fixed level index bug Added generated activities
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -964,7 +964,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1145,7 +1145,7 @@
         <v>5</v>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3" t="n">
         <v>10080</v>
@@ -1159,7 +1159,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>G3</t>
+          <t>G4</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1196,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N4" t="n">
         <v>10080</v>
@@ -1213,7 +1213,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>G4</t>
+          <t>G5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1250,16 +1250,16 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N5" t="n">
         <v>10080</v>
       </c>
       <c r="O5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -1267,7 +1267,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G5</t>
+          <t>G6</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1304,16 +1304,16 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N6" t="n">
         <v>10080</v>
       </c>
       <c r="O6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -1321,7 +1321,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>G6</t>
+          <t>G7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1361,13 +1361,13 @@
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N7" t="n">
         <v>10080</v>
       </c>
       <c r="O7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -1375,7 +1375,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>G7</t>
+          <t>G8</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1412,66 +1412,12 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" t="n">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="N8" t="n">
         <v>10080</v>
       </c>
       <c r="O8" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>17</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>G8</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>45658.25</v>
-      </c>
-      <c r="I9" s="8" t="n">
-        <v>45839.25</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>35</v>
-      </c>
-      <c r="N9" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O9" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1486,7 +1432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1606,7 +1552,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, wjckj0zx007oqzeaenmr3n8zm]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 7unb74jmmueph9796tp69luu10s2g3a0utjvrqd4cdlmn]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1624,7 +1570,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Take_between_1500_and_2500_steps</t>
+          <t>Take_400_steps</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1653,7 +1599,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 1500], [SECRET, EQUAL, bamtcqcnq27x329x284zqrf6z8udrc]</t>
+          <t>[STEPS, STRICTLY_GREATER, 400], [SECRET, EQUAL, pive4rcdhjacqqj9uow5afdveyo8wgak75g2rgvn9ntma]</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -1671,7 +1617,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Take_200_steps</t>
+          <t>Take_a_15-minute_walk_without_stopping</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1687,12 +1633,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1700,7 +1646,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, ecu9yymxf8xssd2oabm9ogv5aqwnw4612kxr]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 9ucpa4nrm5p0u6pgr8yi12m87ol6s]</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -1718,7 +1664,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Take_400_steps</t>
+          <t>Take_between_1500_and_2500_steps</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1747,7 +1693,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 400], [SECRET, EQUAL, 4zpu7w1626ekivqakd3pjro7o31df2nj9u1ol1wxppj9]</t>
+          <t>[STEPS, STRICTLY_GREATER, 1500], [SECRET, EQUAL, eq5e156f5p7tm5rbiu3wjmlgw1oi21joed23oj]</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -1765,7 +1711,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Take_a_15-minute_walk_without_stopping</t>
+          <t>Take_100_steps</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1781,12 +1727,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -1794,7 +1740,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, yjpr8kg73hcggludpy6i5y6gxanmd8du91]</t>
+          <t>[STEPS, STRICTLY_GREATER, 100], [SECRET, EQUAL, nnpywg6plps]</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -1812,7 +1758,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Take_400_steps</t>
+          <t>Take_between_1500_and_2500_steps</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1841,7 +1787,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 400], [SECRET, EQUAL, c929i84vww2b7ewxgf2jryxl]</t>
+          <t>[STEPS, STRICTLY_GREATER, 1500], [SECRET, EQUAL, r1zuir01cz2q54kz8vh8zhi56c]</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -1855,16 +1801,21 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Take_a_15-minute_walk_without_stopping</t>
+          <t>tutorial_video(cognitive_activity)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>http://localhost:5173/api/media/media-for-ai-b7b4437a/a6cf16fb-1b3c-4862-9086-307cb11c2a41.h5p</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1875,12 +1826,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -1888,7 +1839,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, qjbinutffp9vbudwg08efz74qop1uomvts5vpfvsb]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 5hkp2r9msg04o4v]</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -1902,11 +1853,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Put_on_your_walking_shoes_and_take_a_picture_of_them</t>
+          <t>Practice_creative_writing</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1935,11 +1886,11 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, cd8yia2cxvw5n3qf22m6a8f5xo4h228k7hsr97k]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, yjt6zvw2ui9ydxn9cf2gfn]</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1949,21 +1900,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>tutorial_video(cognitive_activity)</t>
+          <t>Take_200_steps</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>http://localhost:5173/api/media/media-for-ai-b7b4437a/a6cf16fb-1b3c-4862-9086-307cb11c2a41.h5p</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1974,12 +1920,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K10" t="n">
@@ -1987,7 +1933,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, pg4gnn75zkgjo47p58fk7iujajfq7u]</t>
+          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, x7dowi6mwc6bvl1zag6vhi]</t>
         </is>
       </c>
       <c r="M10" t="n">
@@ -2005,7 +1951,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Practice_creative_writing</t>
+          <t>Take_200_steps</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2021,12 +1967,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K11" t="n">
@@ -2034,11 +1980,11 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, hsxq1oftbcw4o8mt6cr60tcoexu2lr3ie0pa]</t>
+          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, umrroq3udk9hyhtecou06wgn6j03llswm0bsqnyqb6zbe]</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -2052,7 +1998,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Practice_a_brain_game</t>
+          <t>Practice_learning_a_new_skill</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2081,11 +2027,11 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 17xjf1rufin2iqmjg9rh039oc6dl28]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, weio6e6kt6kpgormjp]</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -2133,7 +2079,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, ejg0ep1ro7v5xmuwisibuzk]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, x29woxz83jhydkb1pcsinnwc6n4ozg4lowpjfcea]</t>
         </is>
       </c>
       <c r="M13" t="n">
@@ -2360,6 +2306,100 @@
         <v>5</v>
       </c>
       <c r="N18" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>8</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Learn_a_new_phrase</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, 0a0ri2ztz0q6w21e6]</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>GameBus Studio</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>8</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Attend_or_watch_a_lecture</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>7</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>GENERAL_ACTIVITY</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> [SECRET, EQUAL, nxw6yfpp4g25ztgqp9]</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>5</v>
+      </c>
+      <c r="N20" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>

<commit_message>
Added graph saving functionality
</commit_message>
<xml_diff>
--- a/website/aples/data/exported1.xlsx
+++ b/website/aples/data/exported1.xlsx
@@ -964,7 +964,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1142,10 +1142,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
         <v>10080</v>
@@ -1159,7 +1159,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>G4</t>
+          <t>G3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1199,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N4" t="n">
         <v>10080</v>
@@ -1213,7 +1213,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>G5</t>
+          <t>G4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1250,16 +1250,16 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N5" t="n">
         <v>10080</v>
       </c>
       <c r="O5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1267,7 +1267,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G6</t>
+          <t>G5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1304,16 +1304,16 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N6" t="n">
         <v>10080</v>
       </c>
       <c r="O6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -1321,7 +1321,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>G7</t>
+          <t>G6</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1358,67 +1358,13 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N7" t="n">
         <v>10080</v>
       </c>
       <c r="O7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>17</v>
-      </c>
-      <c r="B8" t="n">
-        <v>8</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>TASKS_COLLECTION</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>G8</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/3ad4d1db-b854-45cb-bcef-59dbaee47f6e.jpeg</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Generated by AI</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>45658.25</v>
-      </c>
-      <c r="I8" s="8" t="n">
-        <v>45839.25</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>41</v>
-      </c>
-      <c r="N8" t="n">
-        <v>10080</v>
-      </c>
-      <c r="O8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1432,7 +1378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1552,7 +1498,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 7unb74jmmueph9796tp69luu10s2g3a0utjvrqd4cdlmn]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, h5bdjcop3njkonq5a]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -1570,7 +1516,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Take_400_steps</t>
+          <t>Take_200_steps</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1599,7 +1545,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 400], [SECRET, EQUAL, pive4rcdhjacqqj9uow5afdveyo8wgak75g2rgvn9ntma]</t>
+          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, d1vnnashgx3onjzzjzjm]</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -1617,7 +1563,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Take_a_15-minute_walk_without_stopping</t>
+          <t>Take_300_steps</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1633,12 +1579,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1646,7 +1592,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 9ucpa4nrm5p0u6pgr8yi12m87ol6s]</t>
+          <t>[STEPS, STRICTLY_GREATER, 300], [SECRET, EQUAL, pku9reuphqxtk8gzrrnzd7zqef4qu0ffkvc12]</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -1664,7 +1610,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Take_between_1500_and_2500_steps</t>
+          <t>Take_a_25-minute_walk_without_stopping</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1680,12 +1626,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -1693,11 +1639,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 1500], [SECRET, EQUAL, eq5e156f5p7tm5rbiu3wjmlgw1oi21joed23oj]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, jd5fpzwmdo0mmv]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -1707,11 +1653,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Take_100_steps</t>
+          <t>Take_200_steps</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1740,7 +1686,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 100], [SECRET, EQUAL, nnpywg6plps]</t>
+          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, tt5wa0bph8wmc0ncswpxv9yxo1zv8nz873jvierr2dg2ta1j]</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -1754,16 +1700,21 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Take_between_1500_and_2500_steps</t>
+          <t>tutorial_video(cognitive_activity)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>http://localhost:5173/api/media/media-for-ai-b7b4437a/a6cf16fb-1b3c-4862-9086-307cb11c2a41.h5p</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -1774,12 +1725,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>H5P_GENERAL</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -1787,7 +1738,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 1500], [SECRET, EQUAL, r1zuir01cz2q54kz8vh8zhi56c]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, 98mxf58gtj]</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -1801,11 +1752,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>tutorial_video(cognitive_activity)</t>
+          <t>tutorial_video(social_activity)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1815,7 +1766,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>http://localhost:5173/api/media/media-for-ai-b7b4437a/a6cf16fb-1b3c-4862-9086-307cb11c2a41.h5p</t>
+          <t>http://localhost:5173/api/media/media-for-ai-b7b4437a/b7fb3d01-9712-476f-9d53-4876283c73ce.h5p</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1839,7 +1790,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 5hkp2r9msg04o4v]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, nlg7gdk0xywcqlsgk]</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -1853,11 +1804,11 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Practice_creative_writing</t>
+          <t>Take_100_steps</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1873,12 +1824,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>GENERAL_ACTIVITY</t>
+          <t>WALK</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -1886,11 +1837,11 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, yjt6zvw2ui9ydxn9cf2gfn]</t>
+          <t>[STEPS, STRICTLY_GREATER, 100], [SECRET, EQUAL, gtxdio1xesbl]</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1900,11 +1851,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Take_200_steps</t>
+          <t>Practice_learning_a_new_skill</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1920,12 +1871,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K10" t="n">
@@ -1933,11 +1884,11 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, x7dowi6mwc6bvl1zag6vhi]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, jasbuurj8xir62vluedsnu97oybs]</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1947,11 +1898,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Take_200_steps</t>
+          <t>Engage_with_others</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1967,12 +1918,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>WALK</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K11" t="n">
@@ -1980,7 +1931,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[STEPS, STRICTLY_GREATER, 200], [SECRET, EQUAL, umrroq3udk9hyhtecou06wgn6j03llswm0bsqnyqb6zbe]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, yu1o02lpklafy2yygdso457wcm408tc]</t>
         </is>
       </c>
       <c r="M11" t="n">
@@ -1998,7 +1949,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Practice_learning_a_new_skill</t>
+          <t>Enjoy_an_activity_with_a_family_member</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2027,11 +1978,11 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, weio6e6kt6kpgormjp]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, pys1n3czmhjxfcg9zmp76]</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -2041,21 +1992,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>tutorial_video(minigame_activity)</t>
+          <t>Enjoy_an_activity_with_a_family_member</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>http://localhost:5173/api/media/media-for-ai-b7b4437a/ba5eb809-ed8e-4688-acb0-0df598a2c57c.h5p</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -2066,12 +2012,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>H5P_GENERAL</t>
+          <t>GENERAL_ACTIVITY</t>
         </is>
       </c>
       <c r="K13" t="n">
@@ -2079,327 +2025,13 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, x29woxz83jhydkb1pcsinnwc6n4ozg4lowpjfcea]</t>
+          <t xml:space="preserve"> [SECRET, EQUAL, ssiv1kqds4f4s7gbhous]</t>
         </is>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>8</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Confusing Arrows: Buy half heart</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>7</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>ConfusingArrowsData</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>ConfusingArrowsData</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>[MINIGAME_BUY_HALF_HEART, STRICTLY_GREATER, 0],[MINIGAMESTATE_ID, EQUAL, 1]</t>
-        </is>
-      </c>
-      <c r="M14" t="n">
-        <v>-5</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>8</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Confusing Arrows: Score 5 points</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>7</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>ConfusingArrowsData</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>ConfusingArrowsData</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 5],[MINIGAMESTATE_ID, EQUAL, 1]</t>
-        </is>
-      </c>
-      <c r="M15" t="n">
-        <v>10</v>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>8</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Walk 500 meters</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>7</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
-        </is>
-      </c>
-      <c r="M16" t="n">
-        <v>20</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>8</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>PolygonEscape: Score 5 points</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>7</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>PolygonEscape</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>PolygonEscape</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>[MINIGAME_SCORE, STRICTLY_GREATER, 5],[MINIGAMESTATE_ID, EQUAL, 6]</t>
-        </is>
-      </c>
-      <c r="M17" t="n">
-        <v>5</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>8</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Walk 1000 meters</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>7</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>WALK</t>
-        </is>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>[DISTANCE, STRICTLY_GREATER, 499]</t>
-        </is>
-      </c>
-      <c r="M18" t="n">
-        <v>5</v>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>8</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Learn_a_new_phrase</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" t="n">
-        <v>7</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, 0a0ri2ztz0q6w21e6]</t>
-        </is>
-      </c>
-      <c r="M19" t="n">
-        <v>1</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>GameBus Studio</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>8</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Attend_or_watch_a_lecture</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>https://campaigns.healthyw8.gamebus.eu/api/media/HW8-immutable/5ff935d3-d0ae-4dce-bfcd-d2f71bf2ca63.jpeg</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" t="n">
-        <v>7</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>GENERAL_ACTIVITY</t>
-        </is>
-      </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> [SECRET, EQUAL, nxw6yfpp4g25ztgqp9]</t>
-        </is>
-      </c>
-      <c r="M20" t="n">
-        <v>5</v>
-      </c>
-      <c r="N20" t="inlineStr">
         <is>
           <t>GameBus Studio</t>
         </is>

</xml_diff>